<commit_message>
update 0.2.1 discapacidad 1..1 ->0..1 SR
</commit_message>
<xml_diff>
--- a/fhir/ig/tei/0.2.1/StructureDefinition-BundleIniciarLE.xlsx
+++ b/fhir/ig/tei/0.2.1/StructureDefinition-BundleIniciarLE.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-15T11:25:06-04:00</t>
+    <t>2024-07-19T15:20:36-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -573,7 +573,7 @@
     <t>Bundle.entry</t>
   </si>
   <si>
-    <t>9</t>
+    <t>8</t>
   </si>
   <si>
     <t>Entrada en el Bundle: contendrá un recurso o información</t>
@@ -30195,7 +30195,7 @@
       </c>
       <c r="E241" s="2"/>
       <c r="F241" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G241" t="s" s="2">
         <v>87</v>

</xml_diff>